<commit_message>
Calculate a sequence of posteriors given data
* `suite/posteriors-seq`
* `dice/posteriors-seq`
</commit_message>
<xml_diff>
--- a/think-bayes-clj/test/think_bayes/bayes_test_results.xlsx
+++ b/think-bayes-clj/test/think_bayes/bayes_test_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="12">
   <si>
     <t>Hypotheses</t>
   </si>
@@ -99,9 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,19 +769,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:E12"/>
+  <dimension ref="A5:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -789,7 +790,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -806,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -827,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -844,11 +845,11 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E12" si="3">D8/D$12</f>
+        <f t="shared" ref="E8:E11" si="3">D8/D$12</f>
         <v>0.39215686274509809</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -869,7 +870,7 @@
         <v>0.29411764705882359</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>12</v>
       </c>
@@ -890,7 +891,7 @@
         <v>0.19607843137254904</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
@@ -911,12 +912,676 @@
         <v>0.11764705882352945</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D12" s="1">
         <f>SUM(D7:D11)</f>
         <v>8.4999999999999992E-2</v>
       </c>
       <c r="E12" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="1">
+        <v>7</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="C16" s="2">
+        <f>IF(C$15&gt;$A16,0,1/$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <f>B16*C16</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <f>D16/D$21</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <f>IF(F$15&gt;$A16,0,1/$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f>E16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <f>G16/G$21</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f>IF(I$15&gt;$A16,0,1/$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f>H16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <f>J16/J$21</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <f>IF(L$15&gt;$A16,0,1/$A16)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <f>K16*L16</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <f>M16/M$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:B20" si="4">1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:C20" si="5">IF(C$15&gt;$A17,0,1/$A17)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" ref="D17:D20" si="6">B17*C17</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17/D$21</f>
+        <v>0.39215686274509809</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" ref="F17:F21" si="7">IF(F$15&gt;$A17,0,1/$A17)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G21" si="8">E17*F17</f>
+        <v>6.535947712418301E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <f>G17/G$21</f>
+        <v>0.52562417871222067</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" ref="I17:I21" si="9">IF(I$15&gt;$A17,0,1/$A17)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" ref="J17:J21" si="10">H17*I17</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <f>J17/J$21</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L17:L21" si="11">IF(L$15&gt;$A17,0,1/$A17)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" ref="M17:M21" si="12">K17*L17</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <f>M17/M$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="5"/>
+        <v>0.125</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" ref="E18:E20" si="13">D18/D$21</f>
+        <v>0.29411764705882359</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="7"/>
+        <v>0.125</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="8"/>
+        <v>3.6764705882352949E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18:H20" si="14">G18/G$21</f>
+        <v>0.29566360052562418</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="9"/>
+        <v>0.125</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="10"/>
+        <v>3.6957950065703023E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" ref="K18:K20" si="15">J18/J$21</f>
+        <v>0.73513395774341106</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="11"/>
+        <v>0.125</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="12"/>
+        <v>9.1891744717926382E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <f>M18/M$21</f>
+        <v>0.81757400558776516</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="5"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="13"/>
+        <v>0.19607843137254904</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="7"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="8"/>
+        <v>1.6339869281045753E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="14"/>
+        <v>0.13140604467805517</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="9"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="10"/>
+        <v>1.0950503723171263E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="15"/>
+        <v>0.21781746896101062</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="11"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="12"/>
+        <v>1.8151455746750884E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <f>M19/M$21</f>
+        <v>0.16149609986918811</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="13"/>
+        <v>0.11764705882352945</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="7"/>
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="8"/>
+        <v>5.8823529411764731E-3</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="14"/>
+        <v>4.7306176084099885E-2</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="9"/>
+        <v>0.05</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="10"/>
+        <v>2.3653088042049943E-3</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="15"/>
+        <v>4.7048573295578322E-2</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="11"/>
+        <v>0.05</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="12"/>
+        <v>2.3524286647789161E-3</v>
+      </c>
+      <c r="N20" s="2">
+        <f>M20/M$21</f>
+        <v>2.0929894543046793E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
+        <f>SUM(D16:D20)</f>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
+        <f>SUM(G16:G20)</f>
+        <v>0.12434640522875819</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <f>SUM(J16:J20)</f>
+        <v>5.027376259307928E-2</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2">
+        <f>SUM(M16:M20)</f>
+        <v>0.11239562912945618</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
+        <v>4</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
+        <f>N16</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <f>IF(C$23&gt;$A24,0,1/$A24)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <f>B24*C24</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <f>D24/D$29</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <f>IF(F$23&gt;$A24,0,1/$A24)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <f>E24*F24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <f>G24/G$29</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f>IF(I$23&gt;$A24,0,1/$A24)</f>
+        <v>0.25</v>
+      </c>
+      <c r="J24" s="2">
+        <f>H24*I24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <f>J24/J$29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" ref="B25:B28" si="16">N17</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:C28" si="17">IF(C$23&gt;$A25,0,1/$A25)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" ref="D25:D28" si="18">B25*C25</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <f>D25/D$29</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F28" si="19">IF(F$23&gt;$A25,0,1/$A25)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" ref="G25:G28" si="20">E25*F25</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <f>G25/G$29</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" ref="I25:I28" si="21">IF(I$23&gt;$A25,0,1/$A25)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" ref="J25:J28" si="22">H25*I25</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <f>J25/J$29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="16"/>
+        <v>0.81757400558776516</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="18"/>
+        <v>0.10219675069847065</v>
+      </c>
+      <c r="E26" s="2">
+        <f>D26/D$29</f>
+        <v>0.87571253449514574</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="19"/>
+        <v>0.125</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="20"/>
+        <v>0.10946406681189322</v>
+      </c>
+      <c r="H26" s="2">
+        <f>G26/G$29</f>
+        <v>0.91584527196901</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="22"/>
+        <v>0.11448065899612625</v>
+      </c>
+      <c r="K26" s="2">
+        <f>J26/J$29</f>
+        <v>0.94324845367221266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="16"/>
+        <v>0.16149609986918811</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="17"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="18"/>
+        <v>1.3458008322432342E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <f>D27/D$29</f>
+        <v>0.11532016915162407</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="19"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="20"/>
+        <v>9.6100140959686723E-3</v>
+      </c>
+      <c r="H27" s="2">
+        <f>G27/G$29</f>
+        <v>8.0403425797004949E-2</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="21"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="22"/>
+        <v>6.7002854830837451E-3</v>
+      </c>
+      <c r="K27" s="2">
+        <f>J27/J$29</f>
+        <v>5.5206128061290875E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="16"/>
+        <v>2.0929894543046793E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="17"/>
+        <v>0.05</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0464947271523397E-3</v>
+      </c>
+      <c r="E28" s="2">
+        <f>D28/D$29</f>
+        <v>8.9672963532302936E-3</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="19"/>
+        <v>0.05</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="20"/>
+        <v>4.483648176615147E-4</v>
+      </c>
+      <c r="H28" s="2">
+        <f>G28/G$29</f>
+        <v>3.7513022339850655E-3</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="21"/>
+        <v>0.05</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="22"/>
+        <v>1.8756511169925328E-4</v>
+      </c>
+      <c r="K28" s="2">
+        <f>J28/J$29</f>
+        <v>1.5454182664965536E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
+        <f>SUM(D24:D28)</f>
+        <v>0.11670125374805532</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2">
+        <f>SUM(G24:G28)</f>
+        <v>0.11952244572552341</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2">
+        <f>SUM(J24:J28)</f>
+        <v>0.12136850959090924</v>
+      </c>
+      <c r="K29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>